<commit_message>
updated merger list for revision
</commit_message>
<xml_diff>
--- a/container_merger_data20241124.xlsx
+++ b/container_merger_data20241124.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://takudai-my.sharepoint.com/personal/tmatsuda_st_takushoku-u_ac_jp/Documents/デスクトップ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sugur\Dropbox\ship\container_merger_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{DFB493EF-AA3C-4CAE-9F29-4D824C913290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CC58996-6588-442C-880D-2B28CB19A473}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7DB069-9255-4083-8737-D5990005D3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30285" yWindow="885" windowWidth="25050" windowHeight="14115" xr2:uid="{5991EFC2-A57B-4969-A2EE-D8C96D831542}"/>
+    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" xr2:uid="{5991EFC2-A57B-4969-A2EE-D8C96D831542}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="164">
   <si>
     <t xml:space="preserve">Moore-McCormack Lines Inc </t>
     <phoneticPr fontId="2"/>
@@ -825,10 +825,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>GOTO Shipping International Ltd</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>https://www.kaijipress.com/news/container/2017/05/115332/</t>
   </si>
   <si>
@@ -946,6 +942,9 @@
   </si>
   <si>
     <t>https://trid.trb.org/View/320700</t>
+  </si>
+  <si>
+    <t>GOTO Shipping International Ltd</t>
   </si>
 </sst>
 </file>
@@ -956,7 +955,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -964,14 +963,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -979,7 +978,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -988,7 +987,7 @@
       <b/>
       <sz val="11"/>
       <color theme="4"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1031,7 +1030,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5280,21 +5279,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E239ACC6-3156-44C6-98D4-7B7DE0BCB56D}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="41.375" customWidth="1"/>
-    <col min="4" max="5" width="38.125" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="7" width="37.625" customWidth="1"/>
-    <col min="8" max="8" width="70.25" customWidth="1"/>
-    <col min="9" max="9" width="32.75" customWidth="1"/>
+    <col min="3" max="3" width="35.1328125" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.73046875" customWidth="1"/>
+    <col min="7" max="7" width="37.59765625" customWidth="1"/>
+    <col min="8" max="8" width="70.265625" customWidth="1"/>
+    <col min="9" max="9" width="32.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>139</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -5472,13 +5472,13 @@
         <v>2010</v>
       </c>
       <c r="G9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -5810,15 +5810,18 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
       <c r="C27" t="s">
         <v>138</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -5841,7 +5844,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -5861,7 +5864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -5881,7 +5884,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -5901,7 +5904,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -5921,7 +5924,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -5941,7 +5944,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -5961,7 +5964,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -5981,7 +5984,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -6001,7 +6004,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -6024,7 +6027,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -6047,7 +6050,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -6067,7 +6070,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -6087,7 +6090,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -6107,7 +6110,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -6130,7 +6133,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -6156,7 +6159,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -6182,7 +6185,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -6208,7 +6211,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -6234,7 +6237,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>92</v>
       </c>
@@ -6260,7 +6263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -6277,18 +6280,18 @@
         <v>1986</v>
       </c>
       <c r="H57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
@@ -6297,24 +6300,24 @@
         <v>1986</v>
       </c>
       <c r="G58" t="s">
+        <v>156</v>
+      </c>
+      <c r="H58" t="s">
+        <v>155</v>
+      </c>
+      <c r="I58" t="s">
         <v>157</v>
       </c>
-      <c r="H58" t="s">
-        <v>156</v>
-      </c>
-      <c r="I58" t="s">
-        <v>158</v>
-      </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
@@ -6323,21 +6326,21 @@
         <v>1988</v>
       </c>
       <c r="G59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
       <c r="C60" t="s">
+        <v>144</v>
+      </c>
+      <c r="D60" t="s">
         <v>145</v>
-      </c>
-      <c r="D60" t="s">
-        <v>146</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
@@ -6346,21 +6349,21 @@
         <v>1988</v>
       </c>
       <c r="G60" t="s">
+        <v>148</v>
+      </c>
+      <c r="H60" t="s">
         <v>149</v>
       </c>
-      <c r="H60" t="s">
-        <v>150</v>
-      </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>92</v>
       </c>
       <c r="C61" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" t="s">
         <v>143</v>
-      </c>
-      <c r="D61" t="s">
-        <v>144</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
@@ -6369,15 +6372,15 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>92</v>
       </c>
       <c r="C62" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" t="s">
         <v>151</v>
-      </c>
-      <c r="D62" t="s">
-        <v>152</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>19</v>
@@ -6386,21 +6389,21 @@
         <v>1990</v>
       </c>
       <c r="G62" t="s">
+        <v>159</v>
+      </c>
+      <c r="H62" t="s">
         <v>160</v>
       </c>
-      <c r="H62" t="s">
-        <v>161</v>
-      </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>92</v>
       </c>
       <c r="C63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
@@ -6409,7 +6412,7 @@
         <v>1990</v>
       </c>
       <c r="H63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -6429,7 +6432,7 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6445,7 +6448,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>